<commit_message>
Remplissage du Excel de la partie 1 (public/consignes/Rendu-Projet-Part1.xlxs
</commit_message>
<xml_diff>
--- a/public/consignes/Rendu-Projet-Part1.xlsx
+++ b/public/consignes/Rendu-Projet-Part1.xlsx
@@ -1,36 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cedricgagnevin/cloudstation/Documents/Travail/Vacaire LPro/2020/Semestre2-Période 2/Dealabs/Partie 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5C25F5-6795-4A45-AF29-377CAC95E084}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{8D5C25F5-6795-4A45-AF29-377CAC95E084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66192545-82A4-48A1-8EA7-A63993AAFE93}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="17380" windowHeight="16380" xr2:uid="{A58EC350-CF33-BC4F-BC06-897311A7761F}"/>
   </bookViews>
   <sheets>
     <sheet name="Partie 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+  <si>
+    <t>Dealabs - Partie 1</t>
+  </si>
   <si>
     <t>Binome</t>
   </si>
   <si>
-    <t>Prénom NOM</t>
+    <t>Thibault NICOLAS</t>
+  </si>
+  <si>
+    <t>Gabrielle PIERRE</t>
+  </si>
+  <si>
+    <t>Réalisé</t>
   </si>
   <si>
     <t>Fonctionnalité</t>
@@ -39,12 +59,24 @@
     <t>Commentaire</t>
   </si>
   <si>
+    <t>En cours</t>
+  </si>
+  <si>
     <t>Accueil – A la Une</t>
   </si>
   <si>
+    <t>Les deals ne sont pas triés</t>
+  </si>
+  <si>
+    <t>Fait</t>
+  </si>
+  <si>
     <t>Accueil – Hot</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>Bons plans – Hot</t>
   </si>
   <si>
@@ -72,32 +104,26 @@
     <t>Compte – Créer un compte</t>
   </si>
   <si>
-    <t>Réalisé</t>
+    <t>Thème - Bootstrap (ou autre)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BONUS : Déclarer un deal comme « Expiré » </t>
+  </si>
+  <si>
+    <t>BONUS : Gestion des groupes</t>
+  </si>
+  <si>
+    <t>BONUS : Liste des deals d’un groupe</t>
   </si>
   <si>
     <t>BONUS : Compte – Récupération de mot de passe</t>
-  </si>
-  <si>
-    <t>BONUS : Gestion des groupes</t>
-  </si>
-  <si>
-    <t>BONUS : Liste des deals d’un groupe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BONUS : Déclarer un deal comme « Expiré » </t>
-  </si>
-  <si>
-    <t>Dealabs - Partie 1</t>
-  </si>
-  <si>
-    <t>Thème - Bootstrap (ou autre)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,67 +209,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -278,7 +244,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -577,18 +543,18 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.33203125" customWidth="1"/>
+    <col min="2" max="2" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="30.95">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -602,151 +568,173 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="21">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="21">
       <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="18.95">
       <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="18">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="18">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="17.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="17.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:12" ht="17.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="17.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
       <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="17.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="17.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="17.25">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
       <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
       <c r="B20" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
       <c r="B21" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
       <c r="B22" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7:C7 A8:A17 A19:A22">
-    <cfRule type="expression" dxfId="7" priority="7">
+  <conditionalFormatting sqref="A7:B7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>"$A$7=Oui'"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>"$A$7 == 'NON'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:A17 A19:A22">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Non">
-      <formula>NOT(ISERROR(SEARCH("Non",A7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Oui">
-      <formula>NOT(ISERROR(SEARCH("Oui",A7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>"$A$7=Oui'"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>"$A$7 == 'NON'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Non">
-      <formula>NOT(ISERROR(SEARCH("Non",A18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Oui">
-      <formula>NOT(ISERROR(SEARCH("Oui",A18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A22" xr:uid="{84DF03ED-CD0A-5644-9D99-D67FEE6D9C30}">
-      <formula1>"Oui,Non"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>